<commit_message>
Making to track the inventory over time in github
</commit_message>
<xml_diff>
--- a/pn_inventory.xlsx
+++ b/pn_inventory.xlsx
@@ -1592,7 +1592,7 @@
         <v>4.44</v>
       </c>
       <c r="D2">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E2">
         <v>76959</v>
@@ -1948,7 +1948,7 @@
         <v>1.49</v>
       </c>
       <c r="D3">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E3">
         <v>34421</v>
@@ -2304,7 +2304,7 @@
         <v>17.53</v>
       </c>
       <c r="D4">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E4">
         <v>50254</v>
@@ -2657,10 +2657,10 @@
         <v>121</v>
       </c>
       <c r="C5">
-        <v>16.18</v>
+        <v>16.17</v>
       </c>
       <c r="D5">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E5">
         <v>42603</v>
@@ -3013,10 +3013,10 @@
         <v>122</v>
       </c>
       <c r="C6">
-        <v>16.18</v>
+        <v>16.17</v>
       </c>
       <c r="D6">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E6">
         <v>38298</v>
@@ -3372,7 +3372,7 @@
         <v>16.15</v>
       </c>
       <c r="D7">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E7">
         <v>38092</v>
@@ -3728,7 +3728,7 @@
         <v>16.16</v>
       </c>
       <c r="D8">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E8">
         <v>31648</v>
@@ -4084,7 +4084,7 @@
         <v>16.17</v>
       </c>
       <c r="D9">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E9">
         <v>39630</v>
@@ -4437,10 +4437,10 @@
         <v>126</v>
       </c>
       <c r="C10">
-        <v>16.19</v>
+        <v>16.18</v>
       </c>
       <c r="D10">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E10">
         <v>35538</v>
@@ -4793,10 +4793,10 @@
         <v>127</v>
       </c>
       <c r="C11">
-        <v>12.59</v>
+        <v>12.58</v>
       </c>
       <c r="D11">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E11">
         <v>4186</v>
@@ -5152,7 +5152,7 @@
         <v>2.58</v>
       </c>
       <c r="D12">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E12">
         <v>3952</v>
@@ -5508,7 +5508,7 @@
         <v>0.78</v>
       </c>
       <c r="D13">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E13">
         <v>4944</v>
@@ -5861,10 +5861,10 @@
         <v>130</v>
       </c>
       <c r="C14">
-        <v>15.65</v>
+        <v>15.64</v>
       </c>
       <c r="D14">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E14">
         <v>1855</v>
@@ -6217,10 +6217,10 @@
         <v>131</v>
       </c>
       <c r="C15">
-        <v>15.64</v>
+        <v>15.63</v>
       </c>
       <c r="D15">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E15">
         <v>2001</v>
@@ -6573,10 +6573,10 @@
         <v>132</v>
       </c>
       <c r="C16">
-        <v>7.55</v>
+        <v>7.54</v>
       </c>
       <c r="D16">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E16">
         <v>1793</v>
@@ -6932,7 +6932,7 @@
         <v>1.17</v>
       </c>
       <c r="D17">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E17">
         <v>4394</v>
@@ -7288,7 +7288,7 @@
         <v>1.07</v>
       </c>
       <c r="D18">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E18">
         <v>3100</v>
@@ -7644,7 +7644,7 @@
         <v>1.18</v>
       </c>
       <c r="D19">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E19">
         <v>3383</v>
@@ -7997,10 +7997,10 @@
         <v>136</v>
       </c>
       <c r="C20">
-        <v>1.16</v>
+        <v>1.15</v>
       </c>
       <c r="D20">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E20">
         <v>4180</v>
@@ -8356,7 +8356,7 @@
         <v>1.17</v>
       </c>
       <c r="D21">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E21">
         <v>3784</v>
@@ -8712,7 +8712,7 @@
         <v>1.44</v>
       </c>
       <c r="D22">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E22">
         <v>3547</v>
@@ -9068,7 +9068,7 @@
         <v>1.45</v>
       </c>
       <c r="D23">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E23">
         <v>4587</v>
@@ -9424,7 +9424,7 @@
         <v>0.41</v>
       </c>
       <c r="D24">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E24">
         <v>2648</v>
@@ -9780,7 +9780,7 @@
         <v>1.01</v>
       </c>
       <c r="D25">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E25">
         <v>2950</v>
@@ -10136,7 +10136,7 @@
         <v>2.08</v>
       </c>
       <c r="D26">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E26">
         <v>2663</v>
@@ -10492,7 +10492,7 @@
         <v>1.03</v>
       </c>
       <c r="D27">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E27">
         <v>3647</v>
@@ -10848,7 +10848,7 @@
         <v>0.89</v>
       </c>
       <c r="D28">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E28">
         <v>3748</v>
@@ -11204,7 +11204,7 @@
         <v>0.88</v>
       </c>
       <c r="D29">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E29">
         <v>3771</v>
@@ -11560,7 +11560,7 @@
         <v>0.9</v>
       </c>
       <c r="D30">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E30">
         <v>3866</v>
@@ -11916,7 +11916,7 @@
         <v>0.95</v>
       </c>
       <c r="D31">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E31">
         <v>2332</v>
@@ -12272,7 +12272,7 @@
         <v>0.88</v>
       </c>
       <c r="D32">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E32">
         <v>3996</v>
@@ -12628,7 +12628,7 @@
         <v>1.1</v>
       </c>
       <c r="D33">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E33">
         <v>1806</v>
@@ -12984,7 +12984,7 @@
         <v>0.88</v>
       </c>
       <c r="D34">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E34">
         <v>2484</v>
@@ -13340,7 +13340,7 @@
         <v>0.89</v>
       </c>
       <c r="D35">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E35">
         <v>3678</v>
@@ -13696,7 +13696,7 @@
         <v>0.87</v>
       </c>
       <c r="D36">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E36">
         <v>3688</v>
@@ -14052,7 +14052,7 @@
         <v>0.89</v>
       </c>
       <c r="D37">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E37">
         <v>3756</v>
@@ -14408,7 +14408,7 @@
         <v>0.95</v>
       </c>
       <c r="D38">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E38">
         <v>4233</v>
@@ -14764,7 +14764,7 @@
         <v>0.89</v>
       </c>
       <c r="D39">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E39">
         <v>1634</v>
@@ -15120,7 +15120,7 @@
         <v>0.89</v>
       </c>
       <c r="D40">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E40">
         <v>3962</v>
@@ -15476,7 +15476,7 @@
         <v>0.91</v>
       </c>
       <c r="D41">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E41">
         <v>3522</v>
@@ -15832,7 +15832,7 @@
         <v>0.78</v>
       </c>
       <c r="D42">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E42">
         <v>3768</v>
@@ -16188,7 +16188,7 @@
         <v>1.13</v>
       </c>
       <c r="D43">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E43">
         <v>3739</v>
@@ -16544,7 +16544,7 @@
         <v>1.31</v>
       </c>
       <c r="D44">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E44">
         <v>15480</v>
@@ -16900,7 +16900,7 @@
         <v>0.76</v>
       </c>
       <c r="D45">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E45">
         <v>1263</v>
@@ -17256,7 +17256,7 @@
         <v>0.74</v>
       </c>
       <c r="D46">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E46">
         <v>3624</v>
@@ -17612,7 +17612,7 @@
         <v>0.74</v>
       </c>
       <c r="D47">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E47">
         <v>1958</v>
@@ -17968,7 +17968,7 @@
         <v>0.74</v>
       </c>
       <c r="D48">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E48">
         <v>3958</v>
@@ -18324,7 +18324,7 @@
         <v>0.75</v>
       </c>
       <c r="D49">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E49">
         <v>3990</v>
@@ -18680,7 +18680,7 @@
         <v>0.74</v>
       </c>
       <c r="D50">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E50">
         <v>1974</v>
@@ -19036,7 +19036,7 @@
         <v>0.74</v>
       </c>
       <c r="D51">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E51">
         <v>3536</v>
@@ -19392,7 +19392,7 @@
         <v>0.74</v>
       </c>
       <c r="D52">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E52">
         <v>3750</v>
@@ -19748,7 +19748,7 @@
         <v>0.74</v>
       </c>
       <c r="D53">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E53">
         <v>3840</v>
@@ -20104,7 +20104,7 @@
         <v>0.75</v>
       </c>
       <c r="D54">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E54">
         <v>3644</v>
@@ -20460,7 +20460,7 @@
         <v>0.75</v>
       </c>
       <c r="D55">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E55">
         <v>3596</v>
@@ -20816,7 +20816,7 @@
         <v>0.73</v>
       </c>
       <c r="D56">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E56">
         <v>3608</v>
@@ -21172,7 +21172,7 @@
         <v>0.73</v>
       </c>
       <c r="D57">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E57">
         <v>3619</v>
@@ -21528,7 +21528,7 @@
         <v>1.54</v>
       </c>
       <c r="D58">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E58">
         <v>1562</v>
@@ -21884,7 +21884,7 @@
         <v>0.76</v>
       </c>
       <c r="D59">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E59">
         <v>3739</v>
@@ -22240,7 +22240,7 @@
         <v>0.75</v>
       </c>
       <c r="D60">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E60">
         <v>3608</v>
@@ -22596,7 +22596,7 @@
         <v>0.77</v>
       </c>
       <c r="D61">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E61">
         <v>3800</v>
@@ -22952,7 +22952,7 @@
         <v>0.77</v>
       </c>
       <c r="D62">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E62">
         <v>3690</v>
@@ -23308,7 +23308,7 @@
         <v>0.76</v>
       </c>
       <c r="D63">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E63">
         <v>3620</v>
@@ -23664,7 +23664,7 @@
         <v>0.76</v>
       </c>
       <c r="D64">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E64">
         <v>3746</v>
@@ -24020,7 +24020,7 @@
         <v>0.77</v>
       </c>
       <c r="D65">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E65">
         <v>3931</v>
@@ -24376,7 +24376,7 @@
         <v>0.77</v>
       </c>
       <c r="D66">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E66">
         <v>3804</v>
@@ -24732,7 +24732,7 @@
         <v>0.8100000000000001</v>
       </c>
       <c r="D67">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E67">
         <v>1834</v>
@@ -25088,7 +25088,7 @@
         <v>0.78</v>
       </c>
       <c r="D68">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E68">
         <v>3599</v>
@@ -25444,7 +25444,7 @@
         <v>0.83</v>
       </c>
       <c r="D69">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E69">
         <v>1684</v>
@@ -25800,7 +25800,7 @@
         <v>0.78</v>
       </c>
       <c r="D70">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E70">
         <v>3663</v>
@@ -26156,7 +26156,7 @@
         <v>0.78</v>
       </c>
       <c r="D71">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E71">
         <v>3736</v>
@@ -26512,7 +26512,7 @@
         <v>0.78</v>
       </c>
       <c r="D72">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E72">
         <v>3864</v>
@@ -26868,7 +26868,7 @@
         <v>0.83</v>
       </c>
       <c r="D73">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E73">
         <v>1844</v>
@@ -27224,7 +27224,7 @@
         <v>0.83</v>
       </c>
       <c r="D74">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E74">
         <v>3696</v>
@@ -27580,7 +27580,7 @@
         <v>0.82</v>
       </c>
       <c r="D75">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E75">
         <v>3795</v>
@@ -27936,7 +27936,7 @@
         <v>0.8100000000000001</v>
       </c>
       <c r="D76">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E76">
         <v>4320</v>
@@ -28292,7 +28292,7 @@
         <v>0.82</v>
       </c>
       <c r="D77">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E77">
         <v>3728</v>
@@ -28648,7 +28648,7 @@
         <v>0.82</v>
       </c>
       <c r="D78">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E78">
         <v>4044</v>
@@ -29004,7 +29004,7 @@
         <v>0.82</v>
       </c>
       <c r="D79">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E79">
         <v>4295</v>
@@ -29360,7 +29360,7 @@
         <v>0.8100000000000001</v>
       </c>
       <c r="D80">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E80">
         <v>3786</v>
@@ -29716,7 +29716,7 @@
         <v>0.82</v>
       </c>
       <c r="D81">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E81">
         <v>3992</v>
@@ -30072,7 +30072,7 @@
         <v>0.82</v>
       </c>
       <c r="D82">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E82">
         <v>1808</v>
@@ -30428,7 +30428,7 @@
         <v>0.82</v>
       </c>
       <c r="D83">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E83">
         <v>4769</v>
@@ -30784,7 +30784,7 @@
         <v>0.82</v>
       </c>
       <c r="D84">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E84">
         <v>3612</v>
@@ -31140,7 +31140,7 @@
         <v>0.86</v>
       </c>
       <c r="D85">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E85">
         <v>3470</v>
@@ -31496,7 +31496,7 @@
         <v>0.82</v>
       </c>
       <c r="D86">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E86">
         <v>3868</v>
@@ -31852,7 +31852,7 @@
         <v>0.86</v>
       </c>
       <c r="D87">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E87">
         <v>2491</v>
@@ -32208,7 +32208,7 @@
         <v>0.82</v>
       </c>
       <c r="D88">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E88">
         <v>3840</v>
@@ -32564,7 +32564,7 @@
         <v>0.82</v>
       </c>
       <c r="D89">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E89">
         <v>3604</v>
@@ -32920,7 +32920,7 @@
         <v>0.84</v>
       </c>
       <c r="D90">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E90">
         <v>1819</v>
@@ -33276,7 +33276,7 @@
         <v>0.86</v>
       </c>
       <c r="D91">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E91">
         <v>1588</v>
@@ -33632,7 +33632,7 @@
         <v>0.82</v>
       </c>
       <c r="D92">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E92">
         <v>3708</v>
@@ -33988,7 +33988,7 @@
         <v>0.82</v>
       </c>
       <c r="D93">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E93">
         <v>3976</v>
@@ -34344,7 +34344,7 @@
         <v>1.81</v>
       </c>
       <c r="D94">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E94">
         <v>3584</v>
@@ -34700,7 +34700,7 @@
         <v>0.83</v>
       </c>
       <c r="D95">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E95">
         <v>4570</v>
@@ -35056,7 +35056,7 @@
         <v>0.82</v>
       </c>
       <c r="D96">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E96">
         <v>3676</v>
@@ -35412,7 +35412,7 @@
         <v>0.82</v>
       </c>
       <c r="D97">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E97">
         <v>3842</v>
@@ -35768,7 +35768,7 @@
         <v>1.28</v>
       </c>
       <c r="D98">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E98">
         <v>3659</v>
@@ -36124,7 +36124,7 @@
         <v>1.28</v>
       </c>
       <c r="D99">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E99">
         <v>3874</v>
@@ -36480,7 +36480,7 @@
         <v>1.28</v>
       </c>
       <c r="D100">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E100">
         <v>3832</v>
@@ -36827,10 +36827,10 @@
     </row>
     <row r="102" spans="1:118">
       <c r="C102">
-        <v>251.98</v>
+        <v>251.9</v>
       </c>
       <c r="D102">
-        <v>6381</v>
+        <v>6518</v>
       </c>
       <c r="E102">
         <v>705850</v>

</xml_diff>